<commit_message>
Refine prior calculations, calculate lesion multiplicity cross-sectionally and test functions
</commit_message>
<xml_diff>
--- a/_ground_truth/true_params.xlsx
+++ b/_ground_truth/true_params.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selinapi/tutorial_cancer_modeling_des/ground_truth/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selinapi/tutorial_cancer_modeling_des/_ground_truth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9654FD-A16F-3945-9A59-BF22B220AC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FB7F6E-FE4F-944C-AAF1-EF9E2634BC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37020" yWindow="1320" windowWidth="28040" windowHeight="17440" xr2:uid="{3F2257C7-EED0-BA4B-BED8-66F74100CF01}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{3F2257C7-EED0-BA4B-BED8-66F74100CF01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BCD996-C698-8643-A5E1-DD58D05A0C36}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -601,7 +603,8 @@
         <v>24</v>
       </c>
       <c r="E6" s="1">
-        <v>0.08</v>
+        <f>1/16</f>
+        <v>6.25E-2</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Clarify clinical cancer variable names, plot updated IMABC posteriors
</commit_message>
<xml_diff>
--- a/_ground_truth/true_params.xlsx
+++ b/_ground_truth/true_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selinapi/tutorial_cancer_modeling_des/_ground_truth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FB7F6E-FE4F-944C-AAF1-EF9E2634BC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917E0EEF-1D56-4A47-9391-169429BA5786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{3F2257C7-EED0-BA4B-BED8-66F74100CF01}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{3F2257C7-EED0-BA4B-BED8-66F74100CF01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
   <si>
     <t>d_time_H_P</t>
   </si>
@@ -56,24 +56,12 @@
     <t>rate</t>
   </si>
   <si>
-    <t>d_time_P1_C</t>
-  </si>
-  <si>
     <t>d_time_P2_P3</t>
   </si>
   <si>
-    <t>d_time_P2_C</t>
-  </si>
-  <si>
     <t>d_time_P3_P4</t>
   </si>
   <si>
-    <t>d_time_P3_C</t>
-  </si>
-  <si>
-    <t>d_time_P4_C</t>
-  </si>
-  <si>
     <t>exponential</t>
   </si>
   <si>
@@ -92,18 +80,12 @@
     <t>var_id</t>
   </si>
   <si>
-    <t>idx</t>
-  </si>
-  <si>
     <t>d_time_H_L</t>
   </si>
   <si>
     <t>d_time_L_P</t>
   </si>
   <si>
-    <t>d_time_C_Dc</t>
-  </si>
-  <si>
     <t>d_n_L</t>
   </si>
   <si>
@@ -111,6 +93,30 @@
   </si>
   <si>
     <t>lambda</t>
+  </si>
+  <si>
+    <t>d_time_P1_C1</t>
+  </si>
+  <si>
+    <t>d_time_P2_C2</t>
+  </si>
+  <si>
+    <t>d_time_P3_C3</t>
+  </si>
+  <si>
+    <t>d_time_P4_C4</t>
+  </si>
+  <si>
+    <t>d_time_C1_Dc</t>
+  </si>
+  <si>
+    <t>d_time_C2_Dc</t>
+  </si>
+  <si>
+    <t>d_time_C3_Dc</t>
+  </si>
+  <si>
+    <t>d_time_C4_Dc</t>
   </si>
 </sst>
 </file>
@@ -489,381 +495,355 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BCD996-C698-8643-A5E1-DD58D05A0C36}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" t="str">
+        <f>A2&amp;"."&amp;C2</f>
+        <v>d_time_H_L.shape</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>100</v>
+      </c>
+      <c r="E3" t="str">
+        <f>A3&amp;"."&amp;C3</f>
+        <v>d_time_H_L.scale</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" t="str">
+        <f>A4&amp;"."&amp;C4</f>
+        <v>d_time_L_P.shape</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>50</v>
+      </c>
+      <c r="E5" t="str">
+        <f>A5&amp;"."&amp;C5</f>
+        <v>d_time_L_P.scale</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2</v>
-      </c>
-      <c r="F2" t="str">
-        <f>A2&amp;"."&amp;IF(ISBLANK(B2),"",B2&amp;".")&amp;D2</f>
-        <v>d_time_H_L.shape</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1">
-        <v>100</v>
-      </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3" si="0">A3&amp;"."&amp;IF(ISBLANK(B3),"",B3&amp;".")&amp;D3</f>
-        <v>d_time_H_L.scale</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3</v>
-      </c>
-      <c r="F4" t="str">
-        <f>A4&amp;"."&amp;IF(ISBLANK(B4),"",B4&amp;".")&amp;D4</f>
-        <v>d_time_L_P.shape</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1">
-        <v>50</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" ref="F5:F6" si="1">A5&amp;"."&amp;IF(ISBLANK(B5),"",B5&amp;".")&amp;D5</f>
-        <v>d_time_L_P.scale</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="D6" s="1">
         <f>1/16</f>
         <v>6.25E-2</v>
       </c>
-      <c r="F6" t="str">
-        <f t="shared" si="1"/>
+      <c r="E6" t="str">
+        <f>A6&amp;"."&amp;C6</f>
         <v>d_n_L.lambda</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="1">
+      <c r="D7" s="1">
         <v>3</v>
       </c>
-      <c r="F7" t="str">
-        <f>A7&amp;"."&amp;IF(ISBLANK(B7),"",B7&amp;".")&amp;D7</f>
+      <c r="E7" t="str">
+        <f>A7&amp;"."&amp;C7</f>
         <v>d_time_H_P.shape</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="1">
+      <c r="D8" s="1">
         <v>200</v>
       </c>
-      <c r="F8" t="str">
-        <f t="shared" ref="F8:F19" si="2">A8&amp;"."&amp;IF(ISBLANK(B8),"",B8&amp;".")&amp;D8</f>
+      <c r="E8" t="str">
+        <f>A8&amp;"."&amp;C8</f>
         <v>d_time_H_P.scale</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1">
         <v>0.33</v>
       </c>
-      <c r="F9" t="str">
-        <f t="shared" si="2"/>
+      <c r="E9" t="str">
+        <f>A9&amp;"."&amp;C9</f>
         <v>d_time_P1_P2.rate</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="E10" t="str">
+        <f>A10&amp;"."&amp;C10</f>
+        <v>d_time_P1_C1.rate</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.09</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="2"/>
-        <v>d_time_P1_C.rate</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E11" t="str">
+        <f>A11&amp;"."&amp;C11</f>
+        <v>d_time_P2_P3.rate</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E12" t="str">
+        <f>A12&amp;"."&amp;C12</f>
+        <v>d_time_P2_C2.rate</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="2"/>
-        <v>d_time_P2_P3.rate</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="2"/>
-        <v>d_time_P2_C.rate</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="1">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1">
         <v>0.6</v>
       </c>
-      <c r="F13" t="str">
-        <f t="shared" si="2"/>
+      <c r="E13" t="str">
+        <f>A13&amp;"."&amp;C13</f>
         <v>d_time_P3_P4.rate</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="1">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1">
         <v>0.5</v>
       </c>
-      <c r="F14" t="str">
-        <f t="shared" si="2"/>
-        <v>d_time_P3_C.rate</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E14" t="str">
+        <f>A14&amp;"."&amp;C14</f>
+        <v>d_time_P3_C3.rate</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="C15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="1">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
         <v>2</v>
       </c>
-      <c r="F15" t="str">
-        <f t="shared" si="2"/>
-        <v>d_time_P4_C.rate</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E15" t="str">
+        <f>A15&amp;"."&amp;C15</f>
+        <v>d_time_P4_C4.rate</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="1">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1">
         <v>0.05</v>
       </c>
-      <c r="F16" t="str">
-        <f t="shared" si="2"/>
-        <v>d_time_C_Dc.1.rate</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E16" t="str">
+        <f>A16&amp;"."&amp;C16</f>
+        <v>d_time_C1_Dc.rate</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="1">
-        <v>2</v>
+        <v>24</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="1">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1">
         <v>0.08</v>
       </c>
-      <c r="F17" t="str">
-        <f t="shared" si="2"/>
-        <v>d_time_C_Dc.2.rate</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E17" t="str">
+        <f>A17&amp;"."&amp;C17</f>
+        <v>d_time_C2_Dc.rate</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18">
-        <v>3</v>
+        <v>25</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="1">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1">
         <v>0.16</v>
       </c>
-      <c r="F18" t="str">
-        <f t="shared" si="2"/>
-        <v>d_time_C_Dc.3.rate</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E18" t="str">
+        <f>A18&amp;"."&amp;C18</f>
+        <v>d_time_C3_Dc.rate</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="1">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="1">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1">
         <v>0.5</v>
       </c>
-      <c r="F19" t="str">
-        <f t="shared" si="2"/>
-        <v>d_time_C_Dc.4.rate</v>
+      <c r="E19" t="str">
+        <f>A19&amp;"."&amp;C19</f>
+        <v>d_time_C4_Dc.rate</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generate new output figures, update IMABC centers and Sherlock parameters
</commit_message>
<xml_diff>
--- a/_ground_truth/true_params.xlsx
+++ b/_ground_truth/true_params.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selinapi/tutorial_cancer_modeling_des/_ground_truth/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selinapi/Repositories/tutorial_cancer_modeling_des/_ground_truth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917E0EEF-1D56-4A47-9391-169429BA5786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C8646E-9353-1F4F-BD4B-E248CA66418B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{3F2257C7-EED0-BA4B-BED8-66F74100CF01}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" xr2:uid="{3F2257C7-EED0-BA4B-BED8-66F74100CF01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -497,7 +497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BCD996-C698-8643-A5E1-DD58D05A0C36}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -535,7 +537,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="str">
-        <f>A2&amp;"."&amp;C2</f>
+        <f t="shared" ref="E2:E19" si="0">A2&amp;"."&amp;C2</f>
         <v>d_time_H_L.shape</v>
       </c>
     </row>
@@ -553,7 +555,7 @@
         <v>100</v>
       </c>
       <c r="E3" t="str">
-        <f>A3&amp;"."&amp;C3</f>
+        <f t="shared" si="0"/>
         <v>d_time_H_L.scale</v>
       </c>
     </row>
@@ -571,7 +573,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="str">
-        <f>A4&amp;"."&amp;C4</f>
+        <f t="shared" si="0"/>
         <v>d_time_L_P.shape</v>
       </c>
     </row>
@@ -589,7 +591,7 @@
         <v>50</v>
       </c>
       <c r="E5" t="str">
-        <f>A5&amp;"."&amp;C5</f>
+        <f t="shared" si="0"/>
         <v>d_time_L_P.scale</v>
       </c>
     </row>
@@ -608,7 +610,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="E6" t="str">
-        <f>A6&amp;"."&amp;C6</f>
+        <f t="shared" si="0"/>
         <v>d_n_L.lambda</v>
       </c>
     </row>
@@ -626,7 +628,7 @@
         <v>3</v>
       </c>
       <c r="E7" t="str">
-        <f>A7&amp;"."&amp;C7</f>
+        <f t="shared" si="0"/>
         <v>d_time_H_P.shape</v>
       </c>
     </row>
@@ -644,7 +646,7 @@
         <v>200</v>
       </c>
       <c r="E8" t="str">
-        <f>A8&amp;"."&amp;C8</f>
+        <f t="shared" si="0"/>
         <v>d_time_H_P.scale</v>
       </c>
     </row>
@@ -662,7 +664,7 @@
         <v>0.33</v>
       </c>
       <c r="E9" t="str">
-        <f>A9&amp;"."&amp;C9</f>
+        <f t="shared" si="0"/>
         <v>d_time_P1_P2.rate</v>
       </c>
     </row>
@@ -680,7 +682,7 @@
         <v>0.09</v>
       </c>
       <c r="E10" t="str">
-        <f>A10&amp;"."&amp;C10</f>
+        <f t="shared" si="0"/>
         <v>d_time_P1_C1.rate</v>
       </c>
     </row>
@@ -698,7 +700,7 @@
         <v>0.4</v>
       </c>
       <c r="E11" t="str">
-        <f>A11&amp;"."&amp;C11</f>
+        <f t="shared" si="0"/>
         <v>d_time_P2_P3.rate</v>
       </c>
     </row>
@@ -716,7 +718,7 @@
         <v>0.2</v>
       </c>
       <c r="E12" t="str">
-        <f>A12&amp;"."&amp;C12</f>
+        <f t="shared" si="0"/>
         <v>d_time_P2_C2.rate</v>
       </c>
     </row>
@@ -734,7 +736,7 @@
         <v>0.6</v>
       </c>
       <c r="E13" t="str">
-        <f>A13&amp;"."&amp;C13</f>
+        <f t="shared" si="0"/>
         <v>d_time_P3_P4.rate</v>
       </c>
     </row>
@@ -752,7 +754,7 @@
         <v>0.5</v>
       </c>
       <c r="E14" t="str">
-        <f>A14&amp;"."&amp;C14</f>
+        <f t="shared" si="0"/>
         <v>d_time_P3_C3.rate</v>
       </c>
     </row>
@@ -770,7 +772,7 @@
         <v>2</v>
       </c>
       <c r="E15" t="str">
-        <f>A15&amp;"."&amp;C15</f>
+        <f t="shared" si="0"/>
         <v>d_time_P4_C4.rate</v>
       </c>
     </row>
@@ -788,7 +790,7 @@
         <v>0.05</v>
       </c>
       <c r="E16" t="str">
-        <f>A16&amp;"."&amp;C16</f>
+        <f t="shared" si="0"/>
         <v>d_time_C1_Dc.rate</v>
       </c>
     </row>
@@ -806,7 +808,7 @@
         <v>0.08</v>
       </c>
       <c r="E17" t="str">
-        <f>A17&amp;"."&amp;C17</f>
+        <f t="shared" si="0"/>
         <v>d_time_C2_Dc.rate</v>
       </c>
     </row>
@@ -824,7 +826,7 @@
         <v>0.16</v>
       </c>
       <c r="E18" t="str">
-        <f>A18&amp;"."&amp;C18</f>
+        <f t="shared" si="0"/>
         <v>d_time_C3_Dc.rate</v>
       </c>
     </row>
@@ -842,7 +844,7 @@
         <v>0.5</v>
       </c>
       <c r="E19" t="str">
-        <f>A19&amp;"."&amp;C19</f>
+        <f t="shared" si="0"/>
         <v>d_time_C4_Dc.rate</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change cancer progression model structure, check IMABC results, try refining priors for time from lesion to cancer onset
</commit_message>
<xml_diff>
--- a/_ground_truth/true_params.xlsx
+++ b/_ground_truth/true_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selinapi/Repositories/tutorial_cancer_modeling_des/_ground_truth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C8646E-9353-1F4F-BD4B-E248CA66418B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904EB39A-1C62-4D4C-9353-D27C43D82AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" xr2:uid="{3F2257C7-EED0-BA4B-BED8-66F74100CF01}"/>
+    <workbookView xWindow="34880" yWindow="120" windowWidth="30240" windowHeight="17540" xr2:uid="{3F2257C7-EED0-BA4B-BED8-66F74100CF01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
   <si>
     <t>d_time_H_P</t>
   </si>
@@ -56,12 +56,6 @@
     <t>rate</t>
   </si>
   <si>
-    <t>d_time_P2_P3</t>
-  </si>
-  <si>
-    <t>d_time_P3_P4</t>
-  </si>
-  <si>
     <t>exponential</t>
   </si>
   <si>
@@ -95,18 +89,6 @@
     <t>lambda</t>
   </si>
   <si>
-    <t>d_time_P1_C1</t>
-  </si>
-  <si>
-    <t>d_time_P2_C2</t>
-  </si>
-  <si>
-    <t>d_time_P3_C3</t>
-  </si>
-  <si>
-    <t>d_time_P4_C4</t>
-  </si>
-  <si>
     <t>d_time_C1_Dc</t>
   </si>
   <si>
@@ -117,6 +99,15 @@
   </si>
   <si>
     <t>d_time_C4_Dc</t>
+  </si>
+  <si>
+    <t>idx</t>
+  </si>
+  <si>
+    <t>hr_cancer</t>
+  </si>
+  <si>
+    <t>p_cancer</t>
   </si>
 </sst>
 </file>
@@ -495,356 +486,397 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BCD996-C698-8643-A5E1-DD58D05A0C36}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>2</v>
       </c>
-      <c r="E2" t="str">
-        <f t="shared" ref="E2:E19" si="0">A2&amp;"."&amp;C2</f>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F21" si="0">A2&amp;IF(ISBLANK(B2),"",".")&amp;B2&amp;IF(ISBLANK(D2),"",".")&amp;D2</f>
         <v>d_time_H_L.shape</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>100</v>
       </c>
-      <c r="E3" t="str">
+      <c r="F3" t="str">
         <f t="shared" si="0"/>
         <v>d_time_H_L.scale</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>3</v>
       </c>
-      <c r="E4" t="str">
+      <c r="F4" t="str">
         <f t="shared" si="0"/>
         <v>d_time_L_P.shape</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>50</v>
       </c>
-      <c r="E5" t="str">
+      <c r="F5" t="str">
         <f t="shared" si="0"/>
         <v>d_time_L_P.scale</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <f>1/16</f>
         <v>6.25E-2</v>
       </c>
-      <c r="E6" t="str">
+      <c r="F6" t="str">
         <f t="shared" si="0"/>
         <v>d_n_L.lambda</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>3</v>
       </c>
-      <c r="E7" t="str">
+      <c r="F7" t="str">
         <f t="shared" si="0"/>
         <v>d_time_H_P.shape</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>200</v>
       </c>
-      <c r="E8" t="str">
+      <c r="F8" t="str">
         <f t="shared" si="0"/>
         <v>d_time_H_P.scale</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="1">
-        <v>0.33</v>
-      </c>
-      <c r="E9" t="str">
+      <c r="E9" s="1">
+        <f>1/8</f>
+        <v>0.125</v>
+      </c>
+      <c r="F9" t="str">
         <f t="shared" si="0"/>
         <v>d_time_P1_P2.rate</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.09</v>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v>d_time_P1_C1.rate</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F10" t="str">
+        <f>A10&amp;IF(ISBLANK(B10),"",".")&amp;B10&amp;IF(ISBLANK(D10),"",".")&amp;D10</f>
+        <v>hr_cancer.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v>d_time_P2_P3.rate</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" ref="F11:F21" si="1">A11&amp;IF(ISBLANK(B11),"",".")&amp;B11&amp;IF(ISBLANK(D11),"",".")&amp;D11</f>
+        <v>hr_cancer.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>d_time_P2_C2.rate</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="1"/>
+        <v>hr_cancer.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" si="0"/>
-        <v>d_time_P3_P4.rate</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="1"/>
+        <v>hr_cancer.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E14" t="str">
-        <f t="shared" si="0"/>
-        <v>d_time_P3_C3.rate</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>p_cancer.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="1">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="E15" t="str">
-        <f t="shared" si="0"/>
-        <v>d_time_P4_C4.rate</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>p_cancer.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>p_cancer.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1">
+        <f>1-SUM(E14:E16)</f>
+        <v>0.29000000000000004</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
+        <v>p_cancer.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E18" s="1">
         <v>0.05</v>
       </c>
-      <c r="E16" t="str">
-        <f t="shared" si="0"/>
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
         <v>d_time_C1_Dc.rate</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="1" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E19" s="1">
         <v>0.08</v>
       </c>
-      <c r="E17" t="str">
-        <f t="shared" si="0"/>
+      <c r="F19" t="str">
+        <f t="shared" si="1"/>
         <v>d_time_C2_Dc.rate</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="1" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E20" s="1">
         <v>0.16</v>
       </c>
-      <c r="E18" t="str">
-        <f t="shared" si="0"/>
+      <c r="F20" t="str">
+        <f t="shared" si="1"/>
         <v>d_time_C3_Dc.rate</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="1" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E21" s="1">
         <v>0.5</v>
       </c>
-      <c r="E19" t="str">
-        <f t="shared" si="0"/>
+      <c r="F21" t="str">
+        <f t="shared" si="1"/>
         <v>d_time_C4_Dc.rate</v>
       </c>
     </row>

</xml_diff>